<commit_message>
Updated.  Found a defect and a critical failure.
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>RTM</t>
   </si>
@@ -56,14 +56,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Add Account to Database</t>
-  </si>
-  <si>
-    <t>1) Enter Account Details
-2) Click "Add Account To 
-Database"</t>
   </si>
   <si>
     <t>id = hello2
@@ -89,6 +81,84 @@
 3) Log Out
 4) Log In
 5) Check for New Account</t>
+  </si>
+  <si>
+    <t>Defects</t>
+  </si>
+  <si>
+    <t>1) Enter Account Details
+2) Click "Add Account To Database"</t>
+  </si>
+  <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>Register New User and Add
+Account Info</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>Register New User</t>
+  </si>
+  <si>
+    <t>1) Register New User</t>
+  </si>
+  <si>
+    <t>id = new
+pwd = new</t>
+  </si>
+  <si>
+    <t>5b</t>
+  </si>
+  <si>
+    <t>Add Account to Database
+For Existing Users</t>
+  </si>
+  <si>
+    <t>Add Account Info For New
+User</t>
+  </si>
+  <si>
+    <t>1) Log in as new user without 
+any into in database
+2) Add account info</t>
+  </si>
+  <si>
+    <t>id = 444
+pwd = 444</t>
+  </si>
+  <si>
+    <t>Register Multiple Users In
+One Sessions</t>
+  </si>
+  <si>
+    <t>1) Register New User
+2) Log In
+3) Log Out
+4) Register New User</t>
+  </si>
+  <si>
+    <t>Defect_01:
+Must Enter account
+Into multuple times
+to save</t>
+  </si>
+  <si>
+    <t>id = Hello
+pwd = Hello</t>
+  </si>
+  <si>
+    <t>Crash_01:
+Program crash upon second
+account creation</t>
+  </si>
+  <si>
+    <t>Defect</t>
+  </si>
+  <si>
+    <t>Critical Failure</t>
   </si>
 </sst>
 </file>
@@ -104,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +184,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -130,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -141,6 +223,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,133 +529,184 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>6</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>

</xml_diff>

<commit_message>
Updated.  Defect was incorrectly identified.  Crash still occurs.
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>RTM</t>
   </si>
@@ -130,35 +130,30 @@
 pwd = 444</t>
   </si>
   <si>
-    <t>Register Multiple Users In
-One Sessions</t>
-  </si>
-  <si>
     <t>1) Register New User
 2) Log In
 3) Log Out
 4) Register New User</t>
   </si>
   <si>
-    <t>Defect_01:
-Must Enter account
-Into multuple times
-to save</t>
-  </si>
-  <si>
     <t>id = Hello
 pwd = Hello</t>
   </si>
   <si>
+    <t>Defect</t>
+  </si>
+  <si>
+    <t>Critical Failure</t>
+  </si>
+  <si>
+    <t>Register Multiple Users In
+One Sessions or after Log in</t>
+  </si>
+  <si>
     <t>Crash_01:
 Program crash upon second
-account creation</t>
-  </si>
-  <si>
-    <t>Defect</t>
-  </si>
-  <si>
-    <t>Critical Failure</t>
+account creation
+&lt;New Account is successfully created and saved&gt;</t>
   </si>
 </sst>
 </file>
@@ -212,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -228,12 +223,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -241,6 +230,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +530,7 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="6" max="6" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -546,10 +538,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -668,44 +660,42 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>6</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>32</v>
+      <c r="F11" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates to RTM and timeTable
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More Updates to timetable and RTM.  Database changed in testing.
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>RTM</t>
   </si>
@@ -154,6 +154,34 @@
 Program crash upon second
 account creation
 &lt;New Account is successfully created and saved&gt;</t>
+  </si>
+  <si>
+    <t>Repaired Failure</t>
+  </si>
+  <si>
+    <t>Crash_01 Repaired
+Main window is not hidden</t>
+  </si>
+  <si>
+    <t>Attempt to register existing
+User</t>
+  </si>
+  <si>
+    <t>1) Click Register
+2) Enter credentials for existing user
+3) Expect register failure</t>
+  </si>
+  <si>
+    <t>Attempt to read database
+without decryption</t>
+  </si>
+  <si>
+    <t>1) Access database with a database
+viewer without decrypting data</t>
+  </si>
+  <si>
+    <t>Expect incomprehensible
+Information</t>
   </si>
 </sst>
 </file>
@@ -169,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +222,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -207,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -231,6 +265,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -520,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,6 +587,9 @@
       <c r="C1" s="9" t="s">
         <v>31</v>
       </c>
+      <c r="D1" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -698,25 +745,58 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates to Report and RTM
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -159,10 +159,6 @@
     <t>Repaired Failure</t>
   </si>
   <si>
-    <t>Crash_01 Repaired
-Main window is not hidden</t>
-  </si>
-  <si>
     <t>Attempt to register existing
 User</t>
   </si>
@@ -197,15 +193,26 @@
     <t>&lt;delete any existing
 account info&gt;</t>
   </si>
+  <si>
+    <t>Crash_01 Repaired</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -251,52 +258,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyFill="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Style 1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -582,257 +607,271 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="E9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="E10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
         <v>6</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+    <row r="12" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
         <v>6</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="14" t="s">
+      <c r="E12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="1"/>
+      <c r="E15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>

</xml_diff>

<commit_message>
Fixed formatting in word document and RTM
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -201,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +213,13 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -283,39 +290,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -613,10 +620,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -663,7 +670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -681,7 +688,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -699,7 +706,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -715,7 +722,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -733,7 +740,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -745,7 +752,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
@@ -763,7 +770,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
@@ -781,7 +788,7 @@
       </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>6</v>
       </c>
@@ -801,7 +808,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>6</v>
       </c>
@@ -821,7 +828,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>7</v>
       </c>
@@ -837,7 +844,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>8</v>
       </c>
@@ -855,7 +862,7 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Updated documentation and testing procedures
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>RTM</t>
   </si>
@@ -195,6 +195,14 @@
   </si>
   <si>
     <t>Crash_01 Repaired</t>
+  </si>
+  <si>
+    <t>Register Users after Log in</t>
+  </si>
+  <si>
+    <t>1) Log In
+2) Log Out
+3) Register New User</t>
   </si>
 </sst>
 </file>
@@ -613,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,10 +801,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>29</v>

</xml_diff>